<commit_message>
[SYSTEM] 2.0.1 - Vue loading - Vue transition - Edit Calendar Logic - Adding something client need - Working all function - More feature added - Some fixes bug
</commit_message>
<xml_diff>
--- a/public/resource/SampleCalendar.xlsx
+++ b/public/resource/SampleCalendar.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quihuynh/Desktop/project/cuscofftimev2/public/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{026F85A6-2182-6A48-860A-AFBDC4032989}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090C1DB0-92AF-2F4C-A264-FD170D00F994}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14540" xr2:uid="{2AFDDA3F-E581-3943-B063-B85D016CA7F1}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14520" xr2:uid="{2AFDDA3F-E581-3943-B063-B85D016CA7F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,34 +30,121 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Tên Cán Bộ</t>
-  </si>
-  <si>
-    <t>Lớp</t>
-  </si>
-  <si>
-    <t>Từ</t>
-  </si>
-  <si>
-    <t>Đến</t>
-  </si>
-  <si>
-    <t>Số Giờ</t>
-  </si>
-  <si>
-    <t>Ngày</t>
-  </si>
-  <si>
-    <t>Lí Do</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>TRUNG TÂM CÔNG NGHỆ PHẦN MỀM ĐẠI HỌC CẦN THƠ</t>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">ANTHO </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="19"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>U</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">NIVERSITY </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="19"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">OFTWARE </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="19"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>ENTER</t>
+    </r>
+  </si>
+  <si>
+    <t>Khu III, Đại học Cần Thơ - 01 Lý Tự Trọng, TP. Cần Thơ - Tel: 0292.3731072 &amp; Fax: 0292.3731071 - Email: cusc@ctu.edu.vn</t>
+  </si>
+  <si>
+    <t>BẢNG XÁC NHẬN NGHỈ BÙ</t>
+  </si>
+  <si>
+    <t>STT</t>
+  </si>
+  <si>
+    <t>HỌ TÊN</t>
+  </si>
+  <si>
+    <t>LỚP</t>
+  </si>
+  <si>
+    <t>MÔN</t>
+  </si>
+  <si>
+    <t>SỐ GIỜ</t>
+  </si>
+  <si>
+    <t>GHI CHÚ</t>
+  </si>
+  <si>
+    <t>TỔNG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;Tháng&quot;\ mm/yyyy;@"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -65,16 +152,76 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="19"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -82,12 +229,77 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -103,6 +315,64 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>177801</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>12701</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="CUSC- EDU- Mau">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A5581C4-25B3-8B47-92D2-A14686FC206B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12700" y="177801"/>
+          <a:ext cx="596900" cy="368300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -402,38 +672,162 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BF4D30E-6250-5A44-A1D0-F7150AC86C1E}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A1:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" style="1" customWidth="1"/>
+    <col min="8" max="9" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+    </row>
+    <row r="2" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" ht="25" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" ht="25" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="1:9" ht="20" x14ac:dyDescent="0.2">
+      <c r="A6" s="15">
+        <f ca="1">NOW()</f>
+        <v>43600.778939699077</v>
+      </c>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
+      <c r="D7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="6">
+        <f>SUM(E8:E9)</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G11" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A5:F5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>